<commit_message>
delete pip installs and change sheet name to primary
delete pip installs and change sheet name to primary
</commit_message>
<xml_diff>
--- a/signals.xlsx
+++ b/signals.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea7b90198cd15fcb/Documentos/signal-tracker-v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{F9A4A832-0856-40A3-8737-2FA904D08003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{254A4E29-C7AC-4AFF-BE14-23D138F41E9C}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{F9A4A832-0856-40A3-8737-2FA904D08003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DB60797-2003-4F56-95B0-6988BB457DBA}"/>
   <bookViews>
-    <workbookView xWindow="19005" yWindow="4185" windowWidth="36240" windowHeight="11295" activeTab="6" xr2:uid="{7154C1A3-45CB-46F6-AFB1-3A725F3BAFCE}"/>
+    <workbookView xWindow="18675" yWindow="2850" windowWidth="36240" windowHeight="11295" xr2:uid="{7154C1A3-45CB-46F6-AFB1-3A725F3BAFCE}"/>
   </bookViews>
   <sheets>
-    <sheet name="SignalFeed_v2" sheetId="1" r:id="rId1"/>
+    <sheet name="Primary" sheetId="1" r:id="rId1"/>
     <sheet name="ImpactMapping_v1" sheetId="2" r:id="rId2"/>
     <sheet name="Heartbeat_Log" sheetId="3" r:id="rId3"/>
     <sheet name="AllSignalsArchive" sheetId="4" r:id="rId4"/>
@@ -371,6 +371,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5A6209-B4B6-4370-BD52-31F62C9C1739}">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5778CCD1-58CD-489B-A1D5-4A3B2A0F66A2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix excel sheet name for impact engine
</commit_message>
<xml_diff>
--- a/signals.xlsx
+++ b/signals.xlsx
@@ -5013,7 +5013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Newscasts - Timelapse reveals spread of wildfire in California</t>
+          <t>Aid group says worker killed by Israeli military in attack on Gaza HQ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -5186,12 +5186,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Gaza</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-08-04T03:32:35.488000</t>
+          <t>2025-08-04T03:32:07.148000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -5202,40 +5202,40 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Natural Disaster</t>
+          <t>Military Escalation</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-08-04T03:33:58.446586</t>
+          <t>2025-08-04T03:33:58.471599</t>
         </is>
       </c>
       <c r="L2" t="n">
         <v>7</v>
       </c>
       <c r="M2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O2" t="n">
-        <v>6.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>6.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="T2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -5244,25 +5244,25 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2025-08-04T03:33:58.446586</t>
+          <t>2025-08-04T03:33:58.471599</t>
         </is>
       </c>
       <c r="W2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: California)</t>
+          <t>Defense, Oil &amp; Gas, Cybersecurity, Gold/Safe-Havens (Country: Gaza)</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
+          <t>LMT, RTX, XLE, GLD, SFL, HACK</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
+          <t>Defense bullish; region negative; commodities bullish</t>
         </is>
       </c>
       <c r="AA2" t="b">
@@ -5282,7 +5282,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Aid group says worker killed by Israeli military in attack on Gaza HQ</t>
+          <t>Corruption uncovered in Ukrainian defense procurement of military equipment</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -5297,12 +5297,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Gaza</t>
+          <t>Ukrainian</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-08-04T03:32:07.148000</t>
+          <t>2025-08-04T03:12:09.862000</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-08-04T03:33:58.471599</t>
+          <t>2025-08-04T03:33:58.804577</t>
         </is>
       </c>
       <c r="L3" t="n">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2025-08-04T03:33:58.471599</t>
+          <t>2025-08-04T03:33:58.804577</t>
         </is>
       </c>
       <c r="W3" t="b">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Defense, Oil &amp; Gas, Cybersecurity, Gold/Safe-Havens (Country: Gaza)</t>
+          <t>Defense, Oil &amp; Gas, Cybersecurity, Gold/Safe-Havens (Country: Ukrainian)</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -5377,2004 +5377,6 @@
         </is>
       </c>
       <c r="AA3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>The shocking signs and flags at the Harbour Bridge protest - amid warning it could set a new legal precedent</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:32:04.118000</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.498595</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>7</v>
-      </c>
-      <c r="M4" t="n">
-        <v>7</v>
-      </c>
-      <c r="N4" t="n">
-        <v>6</v>
-      </c>
-      <c r="O4" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T4" t="b">
-        <v>0</v>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.498595</t>
-        </is>
-      </c>
-      <c r="W4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Bhopal: Broken Roads Turn Deadly, Locals Protest With Tape</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:31:49.326000</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.522578</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>7</v>
-      </c>
-      <c r="M5" t="n">
-        <v>7</v>
-      </c>
-      <c r="N5" t="n">
-        <v>6</v>
-      </c>
-      <c r="O5" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T5" t="b">
-        <v>0</v>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.522578</t>
-        </is>
-      </c>
-      <c r="W5" t="b">
-        <v>0</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Russia's Krasheninnikov volcano erupts after 600 years, sends ash plume 6 km high</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:30:15.334000</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.541584</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>7</v>
-      </c>
-      <c r="M6" t="n">
-        <v>6</v>
-      </c>
-      <c r="N6" t="n">
-        <v>7</v>
-      </c>
-      <c r="O6" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.541584</t>
-        </is>
-      </c>
-      <c r="W6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Russia)</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Russia's Krasheninnikov Volcano erupts after 600 years, sends ash plume 6 km high</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:30:13.753000</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.564592</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>7</v>
-      </c>
-      <c r="M7" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7</v>
-      </c>
-      <c r="O7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T7" t="b">
-        <v>0</v>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.565584</t>
-        </is>
-      </c>
-      <c r="W7" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Russia)</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Off the cuff: Teachers turn to 'X' for protest</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:30:09.659000</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.592580</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>7</v>
-      </c>
-      <c r="M8" t="n">
-        <v>7</v>
-      </c>
-      <c r="N8" t="n">
-        <v>6</v>
-      </c>
-      <c r="O8" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T8" t="b">
-        <v>0</v>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.592580</t>
-        </is>
-      </c>
-      <c r="W8" t="b">
-        <v>0</v>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Premier holds firm on safety after Gaza bridge protest</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Gaza</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:29:10.241000</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.621600</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>7</v>
-      </c>
-      <c r="M9" t="n">
-        <v>7</v>
-      </c>
-      <c r="N9" t="n">
-        <v>6</v>
-      </c>
-      <c r="O9" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T9" t="b">
-        <v>0</v>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.621600</t>
-        </is>
-      </c>
-      <c r="W9" t="b">
-        <v>0</v>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Gaza)</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Candlelight vigil honors Mount Airy teen who died in flash flood</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:29:08.670000</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.633581</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>7</v>
-      </c>
-      <c r="M10" t="n">
-        <v>6</v>
-      </c>
-      <c r="N10" t="n">
-        <v>7</v>
-      </c>
-      <c r="O10" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T10" t="b">
-        <v>0</v>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.633581</t>
-        </is>
-      </c>
-      <c r="W10" t="b">
-        <v>0</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{"_id":"6890280bd87dc92c4707fba7","slug":"up-flood-situation-in-17-districts-of-the-state-nine-dead-schools-closed-in-many-districts-rain-alert-in-...</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:28:10.832000</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.669577</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>7</v>
-      </c>
-      <c r="M11" t="n">
-        <v>6</v>
-      </c>
-      <c r="N11" t="n">
-        <v>7</v>
-      </c>
-      <c r="O11" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T11" t="b">
-        <v>0</v>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.669577</t>
-        </is>
-      </c>
-      <c r="W11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Minor earthquake occurs on Kyrgyz-Tajik border</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:26:58.068000</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.692579</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>7</v>
-      </c>
-      <c r="M12" t="n">
-        <v>6</v>
-      </c>
-      <c r="N12" t="n">
-        <v>7</v>
-      </c>
-      <c r="O12" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T12" t="b">
-        <v>0</v>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.692579</t>
-        </is>
-      </c>
-      <c r="W12" t="b">
-        <v>0</v>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>August 03, 2025: Bacula Systems SA: How to Choose the Best Enterprise Backup Software in 2025? Best Enterprise Backup Solutions and Tools.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:26:46.306000</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Military Escalation</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.720610</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>7</v>
-      </c>
-      <c r="M13" t="n">
-        <v>9</v>
-      </c>
-      <c r="N13" t="n">
-        <v>9</v>
-      </c>
-      <c r="O13" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="T13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.720610</t>
-        </is>
-      </c>
-      <c r="W13" t="b">
-        <v>0</v>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>Defense, Oil &amp; Gas, Cybersecurity, Gold/Safe-Havens (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>LMT, RTX, XLE, GLD, SFL, HACK</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>Defense bullish; region negative; commodities bullish</t>
-        </is>
-      </c>
-      <c r="AA13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A study in contrasts: Comparing how media outlets covered the Harbour Bridge protest</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:23:13.006000</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.736583</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>7</v>
-      </c>
-      <c r="M14" t="n">
-        <v>7</v>
-      </c>
-      <c r="N14" t="n">
-        <v>6</v>
-      </c>
-      <c r="O14" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T14" t="b">
-        <v>0</v>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.737581</t>
-        </is>
-      </c>
-      <c r="W14" t="b">
-        <v>0</v>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Tropical storm Dexter forms in Atlantic, not forecast to hit land, National Hurricane Center says</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:22:40.243000</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.763574</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>7</v>
-      </c>
-      <c r="M15" t="n">
-        <v>6</v>
-      </c>
-      <c r="N15" t="n">
-        <v>7</v>
-      </c>
-      <c r="O15" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T15" t="b">
-        <v>0</v>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.763574</t>
-        </is>
-      </c>
-      <c r="W15" t="b">
-        <v>0</v>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z15" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Tropical storm Dexter forms in Atlantic, not forecast to hit land, National Hurricane Center says</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:18:11.164000</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Natural Disaster</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.788579</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>7</v>
-      </c>
-      <c r="M16" t="n">
-        <v>6</v>
-      </c>
-      <c r="N16" t="n">
-        <v>7</v>
-      </c>
-      <c r="O16" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T16" t="b">
-        <v>0</v>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.788579</t>
-        </is>
-      </c>
-      <c r="W16" t="b">
-        <v>0</v>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>Insurance, Utilities, Construction, Agriculture (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>MMC, EIX, CAT, DE, ADM</t>
-        </is>
-      </c>
-      <c r="Z16" t="inlineStr">
-        <is>
-          <t>Local negative; Construction bullish (rebuild); Insurance exposure negative</t>
-        </is>
-      </c>
-      <c r="AA16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Corruption uncovered in Ukrainian defense procurement of military equipment</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Ukrainian</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:12:09.862000</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Military Escalation</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.804577</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>7</v>
-      </c>
-      <c r="M17" t="n">
-        <v>9</v>
-      </c>
-      <c r="N17" t="n">
-        <v>9</v>
-      </c>
-      <c r="O17" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="T17" t="b">
-        <v>1</v>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.804577</t>
-        </is>
-      </c>
-      <c r="W17" t="b">
-        <v>1</v>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>Defense, Oil &amp; Gas, Cybersecurity, Gold/Safe-Havens (Country: Ukrainian)</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>LMT, RTX, XLE, GLD, SFL, HACK</t>
-        </is>
-      </c>
-      <c r="Z17" t="inlineStr">
-        <is>
-          <t>Defense bullish; region negative; commodities bullish</t>
-        </is>
-      </c>
-      <c r="AA17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Thousands of Brazilians protest in support of Jair Bolsonaro and against Lula and De Moraes</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:11:52.068000</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.827577</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>7</v>
-      </c>
-      <c r="M18" t="n">
-        <v>7</v>
-      </c>
-      <c r="N18" t="n">
-        <v>6</v>
-      </c>
-      <c r="O18" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T18" t="b">
-        <v>0</v>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.827577</t>
-        </is>
-      </c>
-      <c r="W18" t="b">
-        <v>0</v>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Unknown)</t>
-        </is>
-      </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Premier holds firm on safety after Gaza bridge protest</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Gaza</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:09:30.827000</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.843579</t>
-        </is>
-      </c>
-      <c r="L19" t="n">
-        <v>7</v>
-      </c>
-      <c r="M19" t="n">
-        <v>7</v>
-      </c>
-      <c r="N19" t="n">
-        <v>6</v>
-      </c>
-      <c r="O19" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T19" t="b">
-        <v>0</v>
-      </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.843579</t>
-        </is>
-      </c>
-      <c r="W19" t="b">
-        <v>0</v>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Gaza)</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Premier holds firm on safety after Gaza bridge protest</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Gaza</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:07:41.849000</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Protest</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.862575</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>7</v>
-      </c>
-      <c r="M20" t="n">
-        <v>7</v>
-      </c>
-      <c r="N20" t="n">
-        <v>6</v>
-      </c>
-      <c r="O20" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T20" t="b">
-        <v>0</v>
-      </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.862575</t>
-        </is>
-      </c>
-      <c r="W20" t="b">
-        <v>0</v>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>Energy, Mining, Transportation (Country: Gaza)</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>XLE, OXY, BHP, SFL, TSLA</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>Disruptive: Negative for local ops; bullish if supply constrained elsewhere</t>
-        </is>
-      </c>
-      <c r="AA20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>NEWS_KEYWORD_MATCH</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>LSEG</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Plateau group rebuffs MURIC's allegations on Mutfwang's call for military withdrawal</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>News Headline</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Geopolitical/Economic/Natural</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Mutfwang</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:07:12.771000</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Coup/Political Unrest</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.886585</t>
-        </is>
-      </c>
-      <c r="L21" t="n">
-        <v>7</v>
-      </c>
-      <c r="M21" t="n">
-        <v>8</v>
-      </c>
-      <c r="N21" t="n">
-        <v>9</v>
-      </c>
-      <c r="O21" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="T21" t="b">
-        <v>0</v>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>v1.1</t>
-        </is>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>2025-08-04T03:33:58.888576</t>
-        </is>
-      </c>
-      <c r="W21" t="b">
-        <v>0</v>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>Emerging Markets ETFs, Local Banks, Oil &amp; Gas (Country: Mutfwang)</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>EEM, VALE, TOT, PBR</t>
-        </is>
-      </c>
-      <c r="Z21" t="inlineStr">
-        <is>
-          <t>Risk-off: Negative for local markets; possible safe-haven flows</t>
-        </is>
-      </c>
-      <c r="AA21" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>